<commit_message>
pdf des tests fonctionnels
</commit_message>
<xml_diff>
--- a/dev/TestsFonctionnels/TestsFonctionnelsAPI.xlsx
+++ b/dev/TestsFonctionnels/TestsFonctionnelsAPI.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexi\GitHub\sidekick\dev\TestsFonctionnels\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6CEE8C-A295-4E27-BDC9-7318527454AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Feuille 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>Catégorie</t>
   </si>
@@ -131,33 +140,96 @@
   </si>
   <si>
     <t>La suppression de tous les états d'une commande fonctionne correctement.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Tests fonctionnels de l'API </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>par Alex Lajeunesse</t>
+    </r>
+  </si>
+  <si>
+    <t>*Tous les tests ont été effectués par Alex Lajeunesse le 8 février 2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
-    <font>
-      <sz val="10.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12" x14ac:knownFonts="1">
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-    </font>
-    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
     <font>
       <b/>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -165,7 +237,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -174,59 +246,172 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
-    <border/>
+  <borders count="9">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="26">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -416,319 +601,368 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.57"/>
-    <col customWidth="1" min="2" max="2" width="71.57"/>
-    <col customWidth="1" min="3" max="3" width="35.86"/>
+    <col min="1" max="1" width="25.7109375" customWidth="1"/>
+    <col min="2" max="2" width="60.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C4" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" ht="30.0" customHeight="1">
-      <c r="A2" s="2" t="s">
+    <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" ht="30.0" customHeight="1">
-      <c r="B3" s="2" t="s">
+      <c r="B5" s="23"/>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" ht="30.0" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="5" t="s">
+      <c r="C6" s="12"/>
+    </row>
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="13"/>
+      <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" ht="30.0" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="2" t="s">
+      <c r="C7" s="12"/>
+    </row>
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="13"/>
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" ht="30.0" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="5" t="s">
+      <c r="C8" s="12"/>
+    </row>
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="13"/>
+      <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" ht="30.0" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="5" t="s">
+      <c r="C9" s="12"/>
+    </row>
+    <row r="10" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="13"/>
+      <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" ht="30.0" customHeight="1">
-      <c r="A8" s="6" t="s">
+      <c r="C10" s="12"/>
+    </row>
+    <row r="11" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" ht="30.0" customHeight="1">
-      <c r="A9" s="5" t="s">
+      <c r="B11" s="23"/>
+      <c r="C11" s="14"/>
+    </row>
+    <row r="12" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-    </row>
-    <row r="10" ht="30.0" customHeight="1">
-      <c r="A10" s="7"/>
-      <c r="B10" s="5" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="16"/>
+    </row>
+    <row r="13" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="15"/>
+      <c r="B13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" ht="30.0" customHeight="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="5" t="s">
+      <c r="C13" s="12"/>
+    </row>
+    <row r="14" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="15"/>
+      <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" ht="30.0" customHeight="1">
-      <c r="A12" s="7"/>
-      <c r="B12" s="5" t="s">
+      <c r="C14" s="12"/>
+    </row>
+    <row r="15" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="15"/>
+      <c r="B15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" ht="30.0" customHeight="1">
-      <c r="A13" s="5" t="s">
+      <c r="C15" s="12"/>
+    </row>
+    <row r="16" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" ht="30.0" customHeight="1">
-      <c r="A14" s="3"/>
-      <c r="B14" s="5" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="10"/>
+    </row>
+    <row r="17" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="13"/>
+      <c r="B17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="4"/>
-    </row>
-    <row r="15" ht="30.0" customHeight="1">
-      <c r="A15" s="5" t="s">
+      <c r="C17" s="12"/>
+    </row>
+    <row r="18" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" ht="30.0" customHeight="1">
-      <c r="A16" s="3"/>
-      <c r="B16" s="5" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="10"/>
+    </row>
+    <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="13"/>
+      <c r="B19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" ht="30.0" customHeight="1">
-      <c r="A17" s="3"/>
-      <c r="B17" s="5" t="s">
+      <c r="C19" s="12"/>
+    </row>
+    <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="13"/>
+      <c r="B20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" ht="30.0" customHeight="1">
-      <c r="A18" s="3"/>
-      <c r="B18" s="5" t="s">
+      <c r="C20" s="12"/>
+    </row>
+    <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="13"/>
+      <c r="B21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="4"/>
-    </row>
-    <row r="19" ht="30.0" customHeight="1">
-      <c r="A19" s="3"/>
-      <c r="B19" s="5" t="s">
+      <c r="C21" s="12"/>
+    </row>
+    <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="13"/>
+      <c r="B22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" ht="30.0" customHeight="1">
-      <c r="A20" s="3"/>
-      <c r="B20" s="5" t="s">
+      <c r="C22" s="12"/>
+    </row>
+    <row r="23" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="13"/>
+      <c r="B23" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="4"/>
-    </row>
-    <row r="21" ht="30.0" customHeight="1">
-      <c r="A21" s="3"/>
-      <c r="B21" s="5" t="s">
+      <c r="C23" s="12"/>
+    </row>
+    <row r="24" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="13"/>
+      <c r="B24" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="4"/>
-    </row>
-    <row r="22" ht="30.0" customHeight="1">
-      <c r="A22" s="3"/>
-      <c r="B22" s="5" t="s">
+      <c r="C24" s="12"/>
+    </row>
+    <row r="25" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="13"/>
+      <c r="B25" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="4"/>
-    </row>
-    <row r="23" ht="30.0" customHeight="1">
-      <c r="A23" s="3"/>
-      <c r="B23" s="5" t="s">
+      <c r="C25" s="12"/>
+    </row>
+    <row r="26" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="13"/>
+      <c r="B26" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="4"/>
-    </row>
-    <row r="24" ht="30.0" customHeight="1">
-      <c r="A24" s="3"/>
-      <c r="B24" s="5" t="s">
+      <c r="C26" s="12"/>
+    </row>
+    <row r="27" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="13"/>
+      <c r="B27" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="4"/>
-    </row>
-    <row r="25" ht="30.0" customHeight="1">
-      <c r="A25" s="3"/>
-      <c r="B25" s="5" t="s">
+      <c r="C27" s="12"/>
+    </row>
+    <row r="28" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="13"/>
+      <c r="B28" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="4"/>
-    </row>
-    <row r="26" ht="30.0" customHeight="1">
-      <c r="A26" s="3"/>
-      <c r="B26" s="5" t="s">
+      <c r="C28" s="12"/>
+    </row>
+    <row r="29" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="13"/>
+      <c r="B29" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="4"/>
-    </row>
-    <row r="27" ht="30.0" customHeight="1">
-      <c r="A27" s="5" t="s">
+      <c r="C29" s="12"/>
+    </row>
+    <row r="30" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-    </row>
-    <row r="28" ht="30.0" customHeight="1">
-      <c r="A28" s="3"/>
-      <c r="B28" s="8" t="s">
+      <c r="B30" s="4"/>
+      <c r="C30" s="10"/>
+    </row>
+    <row r="31" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="13"/>
+      <c r="B31" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="4"/>
-    </row>
-    <row r="29" ht="30.0" customHeight="1">
-      <c r="A29" s="3"/>
-      <c r="B29" s="9" t="s">
+      <c r="C31" s="12"/>
+    </row>
+    <row r="32" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="13"/>
+      <c r="B32" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="4"/>
-    </row>
-    <row r="30" ht="30.0" customHeight="1">
-      <c r="A30" s="3"/>
-      <c r="B30" s="9" t="s">
+      <c r="C32" s="12"/>
+    </row>
+    <row r="33" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="13"/>
+      <c r="B33" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="4"/>
-    </row>
-    <row r="31" ht="30.0" customHeight="1">
-      <c r="A31" s="3"/>
-      <c r="B31" s="8" t="s">
+      <c r="C33" s="12"/>
+    </row>
+    <row r="34" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="13"/>
+      <c r="B34" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="4"/>
-    </row>
-    <row r="32" ht="30.0" customHeight="1">
-      <c r="B32" s="10" t="s">
+      <c r="C34" s="12"/>
+    </row>
+    <row r="35" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="11"/>
+      <c r="B35" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="11"/>
-    </row>
-    <row r="33" ht="30.0" customHeight="1">
-      <c r="B33" s="10" t="s">
+      <c r="C35" s="17"/>
+    </row>
+    <row r="36" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="11"/>
+      <c r="B36" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="11"/>
-    </row>
-    <row r="34" ht="30.0" customHeight="1">
-      <c r="B34" s="5" t="s">
+      <c r="C36" s="17"/>
+    </row>
+    <row r="37" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="11"/>
+      <c r="B37" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="11"/>
-    </row>
-    <row r="35" ht="30.0" customHeight="1">
-      <c r="B35" s="2" t="s">
+      <c r="C37" s="17"/>
+    </row>
+    <row r="38" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="11"/>
+      <c r="B38" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="11"/>
-    </row>
-    <row r="36" ht="30.0" customHeight="1">
-      <c r="B36" s="2" t="s">
+      <c r="C38" s="17"/>
+    </row>
+    <row r="39" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="11"/>
+      <c r="B39" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="11"/>
-    </row>
-    <row r="37" ht="30.0" customHeight="1">
-      <c r="A37" s="2" t="s">
+      <c r="C39" s="17"/>
+    </row>
+    <row r="40" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="21" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="38" ht="30.0" customHeight="1">
-      <c r="B38" s="8" t="s">
+      <c r="B40" s="23"/>
+      <c r="C40" s="14"/>
+    </row>
+    <row r="41" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="11"/>
+      <c r="B41" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="11"/>
-    </row>
-    <row r="39" ht="30.0" customHeight="1">
-      <c r="B39" s="10" t="s">
+      <c r="C41" s="17"/>
+    </row>
+    <row r="42" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="11"/>
+      <c r="B42" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C39" s="11"/>
-    </row>
-    <row r="40" ht="30.0" customHeight="1">
-      <c r="B40" s="10" t="s">
+      <c r="C42" s="17"/>
+    </row>
+    <row r="43" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="11"/>
+      <c r="B43" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="11"/>
-    </row>
-    <row r="41" ht="30.0" customHeight="1">
-      <c r="B41" s="2" t="s">
+      <c r="C43" s="17"/>
+    </row>
+    <row r="44" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="11"/>
+      <c r="B44" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="11"/>
-    </row>
-    <row r="42" ht="30.0" customHeight="1">
-      <c r="B42" s="2" t="s">
+      <c r="C44" s="17"/>
+    </row>
+    <row r="45" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="11"/>
+      <c r="B45" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="11"/>
-    </row>
-    <row r="43" ht="30.0" customHeight="1">
-      <c r="B43" s="2" t="s">
+      <c r="C45" s="17"/>
+    </row>
+    <row r="46" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="11"/>
+      <c r="B46" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="11"/>
-    </row>
-    <row r="44" ht="30.0" customHeight="1">
-      <c r="B44" s="2" t="s">
+      <c r="C46" s="17"/>
+    </row>
+    <row r="47" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="18"/>
+      <c r="B47" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="11"/>
+      <c r="C47" s="19"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="86" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>